<commit_message>
HIDAP Status of Creation of FB:  OK!
crop fieldbooks: potato and sweetpotato

statistical designs:
RCBD,CRD,LSD,AUGMENTED, SPLIT PLOT in rcbd, SPLIT PLOT in crd, SPLIT PLOT in lsd
</commit_message>
<xml_diff>
--- a/inst/hidap/templates/potato/template_PTYL.xlsx
+++ b/inst/hidap/templates/potato/template_PTYL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105"/>
   </bookViews>
   <sheets>
     <sheet name="Minimal" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
     <definedName name="trials">#REF!</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1182,10 +1181,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="###0.00"/>
     <numFmt numFmtId="165" formatCode="###0"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -1437,7 +1435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1536,12 +1534,15 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1845,9 +1846,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1904,13 +1905,13 @@
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="50"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="50"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
@@ -2429,7 +2430,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
+      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3765,14 +3766,14 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="49" customWidth="1"/>
     <col min="4" max="4" width="8.140625" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
@@ -3788,7 +3789,7 @@
       <c r="B1" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="47" t="s">
         <v>98</v>
       </c>
       <c r="D1" s="23" t="s">
@@ -3817,7 +3818,7 @@
       <c r="B2" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="42"/>
+      <c r="C2" s="48"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
@@ -3826,10 +3827,10 @@
       <c r="B3" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="s">
@@ -3838,10 +3839,10 @@
       <c r="B4" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3853,7 +3854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
     </sheetView>
@@ -3870,489 +3871,489 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="44" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="45" t="s">
         <v>121</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="45" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="45" t="s">
         <v>123</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="45" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="45" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="45" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="45" t="s">
         <v>127</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="45" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="45" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="46" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="46" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="45" t="s">
         <v>134</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="45" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="45" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="45" t="s">
         <v>138</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="45" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="46" t="s">
+      <c r="A12" s="45" t="s">
         <v>140</v>
       </c>
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="45" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="46" t="s">
+      <c r="A13" s="45" t="s">
         <v>142</v>
       </c>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="45" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="46" t="s">
+      <c r="A14" s="45" t="s">
         <v>144</v>
       </c>
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="45" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="46" t="s">
+      <c r="A15" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="45" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="45" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="46" t="s">
+      <c r="A17" s="45" t="s">
         <v>150</v>
       </c>
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="45" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="45" t="s">
         <v>152</v>
       </c>
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="45" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="45" t="s">
         <v>154</v>
       </c>
-      <c r="B19" s="46" t="s">
+      <c r="B19" s="45" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="45" t="s">
         <v>156</v>
       </c>
-      <c r="B20" s="46" t="s">
+      <c r="B20" s="45" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="45" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="46" t="s">
+      <c r="A22" s="45" t="s">
         <v>160</v>
       </c>
-      <c r="B22" s="46" t="s">
+      <c r="B22" s="45" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="46" t="s">
+      <c r="A23" s="45" t="s">
         <v>162</v>
       </c>
-      <c r="B23" s="46" t="s">
+      <c r="B23" s="45" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="46" t="s">
+      <c r="A24" s="45" t="s">
         <v>164</v>
       </c>
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="45" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="46" t="s">
+      <c r="A25" s="45" t="s">
         <v>166</v>
       </c>
-      <c r="B25" s="46" t="s">
+      <c r="B25" s="45" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="46" t="s">
+      <c r="A26" s="45" t="s">
         <v>168</v>
       </c>
-      <c r="B26" s="46" t="s">
+      <c r="B26" s="45" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="46" t="s">
+      <c r="A27" s="45" t="s">
         <v>170</v>
       </c>
-      <c r="B27" s="46" t="s">
+      <c r="B27" s="45" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="46" t="s">
+      <c r="A28" s="45" t="s">
         <v>172</v>
       </c>
-      <c r="B28" s="46" t="s">
+      <c r="B28" s="45" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="45" t="s">
         <v>174</v>
       </c>
-      <c r="B29" s="46" t="s">
+      <c r="B29" s="45" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="46" t="s">
+      <c r="A30" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="B30" s="46" t="s">
+      <c r="B30" s="45" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="46" t="s">
+      <c r="A31" s="45" t="s">
         <v>178</v>
       </c>
-      <c r="B31" s="46" t="s">
+      <c r="B31" s="45" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="46" t="s">
+      <c r="A32" s="45" t="s">
         <v>180</v>
       </c>
-      <c r="B32" s="46" t="s">
+      <c r="B32" s="45" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="46" t="s">
+      <c r="A33" s="45" t="s">
         <v>182</v>
       </c>
-      <c r="B33" s="46" t="s">
+      <c r="B33" s="45" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="46" t="s">
+      <c r="A34" s="45" t="s">
         <v>184</v>
       </c>
-      <c r="B34" s="46" t="s">
+      <c r="B34" s="45" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="46" t="s">
+      <c r="A35" s="45" t="s">
         <v>186</v>
       </c>
-      <c r="B35" s="46" t="s">
+      <c r="B35" s="45" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="46" t="s">
+      <c r="A36" s="45" t="s">
         <v>188</v>
       </c>
-      <c r="B36" s="46" t="s">
+      <c r="B36" s="45" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="46" t="s">
+      <c r="A37" s="45" t="s">
         <v>190</v>
       </c>
-      <c r="B37" s="46" t="s">
+      <c r="B37" s="45" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="46" t="s">
+      <c r="A38" s="45" t="s">
         <v>192</v>
       </c>
-      <c r="B38" s="46" t="s">
+      <c r="B38" s="45" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="46" t="s">
+      <c r="A39" s="45" t="s">
         <v>194</v>
       </c>
-      <c r="B39" s="46" t="s">
+      <c r="B39" s="45" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="46" t="s">
+      <c r="A40" s="45" t="s">
         <v>196</v>
       </c>
-      <c r="B40" s="46" t="s">
+      <c r="B40" s="45" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="46" t="s">
+      <c r="A41" s="45" t="s">
         <v>198</v>
       </c>
-      <c r="B41" s="46" t="s">
+      <c r="B41" s="45" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="46" t="s">
+      <c r="A42" s="45" t="s">
         <v>200</v>
       </c>
-      <c r="B42" s="46" t="s">
+      <c r="B42" s="45" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="46" t="s">
+      <c r="A43" s="45" t="s">
         <v>202</v>
       </c>
-      <c r="B43" s="46" t="s">
+      <c r="B43" s="45" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="46" t="s">
+      <c r="A44" s="45" t="s">
         <v>204</v>
       </c>
-      <c r="B44" s="46" t="s">
+      <c r="B44" s="45" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="46" t="s">
+      <c r="A45" s="45" t="s">
         <v>206</v>
       </c>
-      <c r="B45" s="46" t="s">
+      <c r="B45" s="45" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="46" t="s">
+      <c r="A46" s="45" t="s">
         <v>208</v>
       </c>
-      <c r="B46" s="46" t="s">
+      <c r="B46" s="45" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="46" t="s">
+      <c r="A47" s="45" t="s">
         <v>210</v>
       </c>
-      <c r="B47" s="46" t="s">
+      <c r="B47" s="45" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="46" t="s">
+      <c r="A48" s="45" t="s">
         <v>212</v>
       </c>
-      <c r="B48" s="46" t="s">
+      <c r="B48" s="45" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="46" t="s">
+      <c r="A49" s="45" t="s">
         <v>214</v>
       </c>
-      <c r="B49" s="46" t="s">
+      <c r="B49" s="45" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="46" t="s">
+      <c r="A50" s="45" t="s">
         <v>216</v>
       </c>
-      <c r="B50" s="46" t="s">
+      <c r="B50" s="45" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="46" t="s">
+      <c r="A51" s="45" t="s">
         <v>218</v>
       </c>
-      <c r="B51" s="46" t="s">
+      <c r="B51" s="45" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="46" t="s">
+      <c r="A52" s="45" t="s">
         <v>220</v>
       </c>
-      <c r="B52" s="46" t="s">
+      <c r="B52" s="45" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="46" t="s">
+      <c r="A53" s="45" t="s">
         <v>222</v>
       </c>
-      <c r="B53" s="46" t="s">
+      <c r="B53" s="45" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="46" t="s">
+      <c r="A54" s="45" t="s">
         <v>224</v>
       </c>
-      <c r="B54" s="46" t="s">
+      <c r="B54" s="45" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="46" t="s">
+      <c r="A55" s="45" t="s">
         <v>226</v>
       </c>
-      <c r="B55" s="46" t="s">
+      <c r="B55" s="45" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="46" t="s">
+      <c r="A56" s="45" t="s">
         <v>228</v>
       </c>
-      <c r="B56" s="46" t="s">
+      <c r="B56" s="45" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" s="46" t="s">
+      <c r="A57" s="45" t="s">
         <v>230</v>
       </c>
-      <c r="B57" s="46" t="s">
+      <c r="B57" s="45" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" s="46" t="s">
+      <c r="A58" s="45" t="s">
         <v>232</v>
       </c>
-      <c r="B58" s="46" t="s">
+      <c r="B58" s="45" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="46" t="s">
+      <c r="A59" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="B59" s="46" t="s">
+      <c r="B59" s="45" t="s">
         <v>234</v>
       </c>
     </row>

</xml_diff>

<commit_message>
load library shinyBS load library rpivotTable 6-24-2015
</commit_message>
<xml_diff>
--- a/inst/hidap/templates/potato/template_PTYL.xlsx
+++ b/inst/hidap/templates/potato/template_PTYL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Minimal" sheetId="1" r:id="rId1"/>
@@ -317,20 +317,6 @@
     <t>Male code</t>
   </si>
   <si>
-    <r>
-      <t>Seed source</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
     <t>References to silmultaneous trials</t>
   </si>
   <si>
@@ -1175,6 +1161,9 @@
   </si>
   <si>
     <t>Flowering</t>
+  </si>
+  <si>
+    <t>Seed source</t>
   </si>
 </sst>
 </file>
@@ -1185,7 +1174,7 @@
     <numFmt numFmtId="164" formatCode="###0.00"/>
     <numFmt numFmtId="165" formatCode="###0"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1258,12 +1247,6 @@
       <color rgb="FF000000"/>
       <name val="Courier New"/>
       <family val="3"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="9"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1846,7 +1829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B7" sqref="B7:B8"/>
     </sheetView>
@@ -1876,7 +1859,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2080,7 +2063,7 @@
         <v>44</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2101,22 +2084,22 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="16" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="16" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="16" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -2182,16 +2165,16 @@
     </row>
     <row r="7" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B7" s="27"/>
     </row>
     <row r="8" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="B8" s="27" t="s">
         <v>316</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -2212,10 +2195,10 @@
     </row>
     <row r="11" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="B11" s="29" t="s">
         <v>318</v>
-      </c>
-      <c r="B11" s="29" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2228,7 +2211,7 @@
     </row>
     <row r="13" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B13" s="29"/>
     </row>
@@ -2428,9 +2411,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+      <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2480,13 +2463,13 @@
         <v>94</v>
       </c>
       <c r="K1" s="36" t="s">
+        <v>377</v>
+      </c>
+      <c r="L1" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="M1" s="36" t="s">
         <v>96</v>
-      </c>
-      <c r="M1" s="36" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2516,69 +2499,69 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>235</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="C1" s="23" t="s">
         <v>236</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="D1" s="23" t="s">
         <v>237</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="E1" s="23" t="s">
         <v>238</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="F1" s="23" t="s">
         <v>239</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="G1" s="23" t="s">
         <v>240</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="H1" s="23" t="s">
         <v>241</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="I1" s="23" t="s">
         <v>242</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="J1" s="23" t="s">
         <v>243</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="K1" s="23" t="s">
         <v>244</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="L1" s="23" t="s">
         <v>245</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="M1" s="23" t="s">
         <v>246</v>
-      </c>
-      <c r="M1" s="23" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
+        <v>248</v>
+      </c>
+      <c r="B3" s="23" t="s">
         <v>249</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>250</v>
       </c>
       <c r="C3" s="23"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C4" s="23"/>
     </row>
@@ -2587,7 +2570,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C5" s="23"/>
     </row>
@@ -2596,434 +2579,434 @@
         <v>24</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C6" s="23"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
+        <v>253</v>
+      </c>
+      <c r="B7" s="23" t="s">
         <v>254</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>255</v>
       </c>
       <c r="C7" s="23"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
+        <v>255</v>
+      </c>
+      <c r="B8" s="23" t="s">
         <v>256</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>257</v>
       </c>
       <c r="C8" s="23"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
+        <v>257</v>
+      </c>
+      <c r="B9" s="23" t="s">
         <v>258</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>259</v>
       </c>
       <c r="C9" s="23"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C10" s="23"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
+        <v>260</v>
+      </c>
+      <c r="B11" s="23" t="s">
         <v>261</v>
       </c>
-      <c r="B11" s="23" t="s">
-        <v>262</v>
-      </c>
       <c r="C11" s="23" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
+        <v>262</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>262</v>
+      </c>
+      <c r="C12" s="23" t="s">
         <v>263</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>263</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
+        <v>323</v>
+      </c>
+      <c r="B14" s="23" t="s">
         <v>324</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>325</v>
       </c>
       <c r="C14" s="23"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
+        <v>265</v>
+      </c>
+      <c r="B15" s="23" t="s">
         <v>266</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="C15" s="23" t="s">
         <v>267</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
+        <v>268</v>
+      </c>
+      <c r="B16" s="23" t="s">
         <v>269</v>
       </c>
-      <c r="B16" s="23" t="s">
-        <v>270</v>
-      </c>
       <c r="C16" s="23" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
+        <v>271</v>
+      </c>
+      <c r="B18" s="23" t="s">
         <v>272</v>
       </c>
-      <c r="B18" s="23" t="s">
-        <v>273</v>
-      </c>
       <c r="C18" s="23" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C20" s="23"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
+        <v>274</v>
+      </c>
+      <c r="B21" s="23" t="s">
         <v>275</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="C21" s="23" t="s">
         <v>276</v>
-      </c>
-      <c r="C21" s="23" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
+        <v>277</v>
+      </c>
+      <c r="B22" s="23" t="s">
         <v>278</v>
       </c>
-      <c r="B22" s="23" t="s">
-        <v>279</v>
-      </c>
       <c r="C22" s="23" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="23" t="s">
+        <v>279</v>
+      </c>
+      <c r="B23" s="23" t="s">
         <v>280</v>
       </c>
-      <c r="B23" s="23" t="s">
-        <v>281</v>
-      </c>
       <c r="C23" s="23" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="23" t="s">
+        <v>281</v>
+      </c>
+      <c r="B24" s="23" t="s">
         <v>282</v>
       </c>
-      <c r="B24" s="23" t="s">
-        <v>283</v>
-      </c>
       <c r="C24" s="23" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="23" t="s">
+        <v>283</v>
+      </c>
+      <c r="B25" s="23" t="s">
         <v>284</v>
       </c>
-      <c r="B25" s="23" t="s">
-        <v>285</v>
-      </c>
       <c r="C25" s="23" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="23" t="s">
+        <v>285</v>
+      </c>
+      <c r="B26" s="23" t="s">
         <v>286</v>
       </c>
-      <c r="B26" s="23" t="s">
-        <v>287</v>
-      </c>
       <c r="C26" s="23" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C27" s="23"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="23" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C28" s="23"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="B30" s="23" t="s">
         <v>291</v>
       </c>
-      <c r="B30" s="23" t="s">
-        <v>292</v>
-      </c>
       <c r="C30" s="23" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="23" t="s">
+        <v>292</v>
+      </c>
+      <c r="B31" s="23" t="s">
         <v>293</v>
       </c>
-      <c r="B31" s="23" t="s">
-        <v>294</v>
-      </c>
       <c r="C31" s="23" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="23" t="s">
+        <v>294</v>
+      </c>
+      <c r="B32" s="23" t="s">
         <v>295</v>
       </c>
-      <c r="B32" s="23" t="s">
-        <v>296</v>
-      </c>
       <c r="C32" s="23" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="23" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="23" t="s">
+        <v>297</v>
+      </c>
+      <c r="B34" s="23" t="s">
         <v>298</v>
       </c>
-      <c r="B34" s="23" t="s">
-        <v>299</v>
-      </c>
       <c r="C34" s="23" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="23" t="s">
+        <v>328</v>
+      </c>
+      <c r="B35" s="23" t="s">
         <v>329</v>
-      </c>
-      <c r="B35" s="23" t="s">
-        <v>330</v>
       </c>
       <c r="C35" s="23"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="23" t="s">
+        <v>330</v>
+      </c>
+      <c r="B36" s="23" t="s">
         <v>331</v>
-      </c>
-      <c r="B36" s="23" t="s">
-        <v>332</v>
       </c>
       <c r="C36" s="23"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="23" t="s">
+        <v>332</v>
+      </c>
+      <c r="B37" s="23" t="s">
         <v>333</v>
-      </c>
-      <c r="B37" s="23" t="s">
-        <v>334</v>
       </c>
       <c r="C37" s="23"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="B38" s="23" t="s">
         <v>335</v>
-      </c>
-      <c r="B38" s="23" t="s">
-        <v>336</v>
       </c>
       <c r="C38" s="23"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="23" t="s">
+        <v>336</v>
+      </c>
+      <c r="B39" s="23" t="s">
         <v>337</v>
-      </c>
-      <c r="B39" s="23" t="s">
-        <v>338</v>
       </c>
       <c r="C39" s="23"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="B40" s="23" t="s">
         <v>300</v>
-      </c>
-      <c r="B40" s="23" t="s">
-        <v>301</v>
       </c>
       <c r="C40" s="23"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="23" t="s">
+        <v>301</v>
+      </c>
+      <c r="B41" s="23" t="s">
         <v>302</v>
-      </c>
-      <c r="B41" s="23" t="s">
-        <v>303</v>
       </c>
       <c r="C41" s="23"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="23" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C42" s="23"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="23" t="s">
+        <v>304</v>
+      </c>
+      <c r="B43" s="23" t="s">
         <v>305</v>
-      </c>
-      <c r="B43" s="23" t="s">
-        <v>306</v>
       </c>
       <c r="C43" s="23"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="B44" s="23" t="s">
         <v>307</v>
-      </c>
-      <c r="B44" s="23" t="s">
-        <v>308</v>
       </c>
       <c r="C44" s="23"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="23" t="s">
+        <v>339</v>
+      </c>
+      <c r="B45" s="23" t="s">
         <v>340</v>
-      </c>
-      <c r="B45" s="23" t="s">
-        <v>341</v>
       </c>
       <c r="C45" s="23"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="23" t="s">
+        <v>341</v>
+      </c>
+      <c r="B46" s="23" t="s">
         <v>342</v>
-      </c>
-      <c r="B46" s="23" t="s">
-        <v>343</v>
       </c>
       <c r="C46" s="23"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="23" t="s">
+        <v>343</v>
+      </c>
+      <c r="B47" s="23" t="s">
         <v>344</v>
-      </c>
-      <c r="B47" s="23" t="s">
-        <v>345</v>
       </c>
       <c r="C47" s="23"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="23" t="s">
+        <v>345</v>
+      </c>
+      <c r="B48" s="23" t="s">
         <v>346</v>
-      </c>
-      <c r="B48" s="23" t="s">
-        <v>347</v>
       </c>
       <c r="C48" s="23"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="23" t="s">
+        <v>347</v>
+      </c>
+      <c r="B49" s="23" t="s">
         <v>348</v>
-      </c>
-      <c r="B49" s="23" t="s">
-        <v>349</v>
       </c>
       <c r="C49" s="23"/>
     </row>
@@ -3049,88 +3032,88 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="37" t="s">
+        <v>349</v>
+      </c>
+      <c r="B1" s="37" t="s">
         <v>350</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="C1" s="37" t="s">
         <v>351</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="D1" s="37" t="s">
+        <v>247</v>
+      </c>
+      <c r="E1" s="37" t="s">
         <v>352</v>
       </c>
-      <c r="D1" s="37" t="s">
-        <v>248</v>
-      </c>
-      <c r="E1" s="37" t="s">
+      <c r="F1" s="37" t="s">
         <v>353</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="G1" s="37" t="s">
         <v>354</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="H1" s="37" t="s">
         <v>355</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="I1" s="37" t="s">
         <v>356</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="J1" s="37" t="s">
         <v>357</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="K1" s="37" t="s">
         <v>358</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="L1" s="37" t="s">
         <v>359</v>
       </c>
-      <c r="L1" s="37" t="s">
+      <c r="M1" s="37" t="s">
         <v>360</v>
       </c>
-      <c r="M1" s="37" t="s">
+      <c r="N1" s="37" t="s">
         <v>361</v>
       </c>
-      <c r="N1" s="37" t="s">
+      <c r="O1" s="37" t="s">
         <v>362</v>
       </c>
-      <c r="O1" s="37" t="s">
+      <c r="P1" s="37" t="s">
         <v>363</v>
       </c>
-      <c r="P1" s="37" t="s">
+      <c r="Q1" s="37" t="s">
         <v>364</v>
       </c>
-      <c r="Q1" s="37" t="s">
+      <c r="R1" s="37" t="s">
         <v>365</v>
       </c>
-      <c r="R1" s="37" t="s">
+      <c r="S1" s="37" t="s">
         <v>366</v>
       </c>
-      <c r="S1" s="37" t="s">
+      <c r="T1" s="37" t="s">
         <v>367</v>
       </c>
-      <c r="T1" s="37" t="s">
+      <c r="U1" s="37" t="s">
         <v>368</v>
       </c>
-      <c r="U1" s="37" t="s">
+      <c r="V1" s="37" t="s">
         <v>369</v>
       </c>
-      <c r="V1" s="37" t="s">
+      <c r="W1" s="37" t="s">
         <v>370</v>
       </c>
-      <c r="W1" s="37" t="s">
+      <c r="X1" s="37" t="s">
         <v>371</v>
       </c>
-      <c r="X1" s="37" t="s">
+      <c r="Y1" s="37" t="s">
         <v>372</v>
       </c>
-      <c r="Y1" s="37" t="s">
+      <c r="Z1" s="37" t="s">
         <v>373</v>
       </c>
-      <c r="Z1" s="37" t="s">
+      <c r="AA1" s="37" t="s">
         <v>374</v>
       </c>
-      <c r="AA1" s="37" t="s">
+      <c r="AB1" s="38" t="s">
         <v>375</v>
-      </c>
-      <c r="AB1" s="38" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
@@ -3784,48 +3767,48 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="C1" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="47" t="s">
-        <v>98</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" s="23" t="s">
+      <c r="F1" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="G1" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="H1" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="I1" s="23" t="s">
         <v>108</v>
-      </c>
-      <c r="I1" s="23" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="41" t="s">
         <v>110</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>111</v>
       </c>
       <c r="C2" s="48"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="41" t="s">
         <v>112</v>
-      </c>
-      <c r="B3" s="41" t="s">
-        <v>113</v>
       </c>
       <c r="F3" s="42"/>
       <c r="G3" s="42"/>
@@ -3834,10 +3817,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F4" s="42"/>
       <c r="G4" s="42"/>
@@ -3872,489 +3855,489 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="43" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="C1" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="D1" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="E1" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="F1" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="G1" s="44" t="s">
         <v>119</v>
-      </c>
-      <c r="G1" s="44" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="45" t="s">
         <v>121</v>
-      </c>
-      <c r="B2" s="45" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="45" t="s">
         <v>123</v>
-      </c>
-      <c r="B3" s="45" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="45" t="s">
         <v>125</v>
-      </c>
-      <c r="B4" s="45" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" s="45" t="s">
         <v>127</v>
-      </c>
-      <c r="B5" s="45" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="45" t="s">
         <v>129</v>
-      </c>
-      <c r="B6" s="45" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="45" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B7" s="46" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8" s="46" t="s">
         <v>132</v>
-      </c>
-      <c r="B8" s="46" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="45" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="45" t="s">
         <v>134</v>
-      </c>
-      <c r="B9" s="45" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="45" t="s">
         <v>136</v>
-      </c>
-      <c r="B10" s="45" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="45" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" s="45" t="s">
         <v>138</v>
-      </c>
-      <c r="B11" s="45" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" s="45" t="s">
         <v>140</v>
-      </c>
-      <c r="B12" s="45" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="45" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13" s="45" t="s">
         <v>142</v>
-      </c>
-      <c r="B13" s="45" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="45" t="s">
+        <v>143</v>
+      </c>
+      <c r="B14" s="45" t="s">
         <v>144</v>
-      </c>
-      <c r="B14" s="45" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="B15" s="45" t="s">
         <v>146</v>
-      </c>
-      <c r="B15" s="45" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="45" t="s">
+        <v>147</v>
+      </c>
+      <c r="B16" s="45" t="s">
         <v>148</v>
-      </c>
-      <c r="B16" s="45" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="B17" s="45" t="s">
         <v>150</v>
-      </c>
-      <c r="B17" s="45" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B18" s="45" t="s">
         <v>152</v>
-      </c>
-      <c r="B18" s="45" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="B19" s="45" t="s">
         <v>154</v>
-      </c>
-      <c r="B19" s="45" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="B20" s="45" t="s">
         <v>156</v>
-      </c>
-      <c r="B20" s="45" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="45" t="s">
+        <v>157</v>
+      </c>
+      <c r="B21" s="45" t="s">
         <v>158</v>
-      </c>
-      <c r="B21" s="45" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="45" t="s">
+        <v>159</v>
+      </c>
+      <c r="B22" s="45" t="s">
         <v>160</v>
-      </c>
-      <c r="B22" s="45" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="45" t="s">
+        <v>161</v>
+      </c>
+      <c r="B23" s="45" t="s">
         <v>162</v>
-      </c>
-      <c r="B23" s="45" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="45" t="s">
+        <v>163</v>
+      </c>
+      <c r="B24" s="45" t="s">
         <v>164</v>
-      </c>
-      <c r="B24" s="45" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="45" t="s">
+        <v>165</v>
+      </c>
+      <c r="B25" s="45" t="s">
         <v>166</v>
-      </c>
-      <c r="B25" s="45" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="45" t="s">
+        <v>167</v>
+      </c>
+      <c r="B26" s="45" t="s">
         <v>168</v>
-      </c>
-      <c r="B26" s="45" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="45" t="s">
+        <v>169</v>
+      </c>
+      <c r="B27" s="45" t="s">
         <v>170</v>
-      </c>
-      <c r="B27" s="45" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="45" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B28" s="45" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="45" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B29" s="45" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="B30" s="45" t="s">
         <v>176</v>
-      </c>
-      <c r="B30" s="45" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="B31" s="45" t="s">
         <v>178</v>
-      </c>
-      <c r="B31" s="45" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="45" t="s">
+        <v>179</v>
+      </c>
+      <c r="B32" s="45" t="s">
         <v>180</v>
-      </c>
-      <c r="B32" s="45" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="45" t="s">
+        <v>181</v>
+      </c>
+      <c r="B33" s="45" t="s">
         <v>182</v>
-      </c>
-      <c r="B33" s="45" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="45" t="s">
+        <v>183</v>
+      </c>
+      <c r="B34" s="45" t="s">
         <v>184</v>
-      </c>
-      <c r="B34" s="45" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="45" t="s">
+        <v>185</v>
+      </c>
+      <c r="B35" s="45" t="s">
         <v>186</v>
-      </c>
-      <c r="B35" s="45" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="45" t="s">
+        <v>187</v>
+      </c>
+      <c r="B36" s="45" t="s">
         <v>188</v>
-      </c>
-      <c r="B36" s="45" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="45" t="s">
+        <v>189</v>
+      </c>
+      <c r="B37" s="45" t="s">
         <v>190</v>
-      </c>
-      <c r="B37" s="45" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="45" t="s">
+        <v>191</v>
+      </c>
+      <c r="B38" s="45" t="s">
         <v>192</v>
-      </c>
-      <c r="B38" s="45" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="45" t="s">
+        <v>193</v>
+      </c>
+      <c r="B39" s="45" t="s">
         <v>194</v>
-      </c>
-      <c r="B39" s="45" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="45" t="s">
+        <v>195</v>
+      </c>
+      <c r="B40" s="45" t="s">
         <v>196</v>
-      </c>
-      <c r="B40" s="45" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="45" t="s">
+        <v>197</v>
+      </c>
+      <c r="B41" s="45" t="s">
         <v>198</v>
-      </c>
-      <c r="B41" s="45" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="45" t="s">
+        <v>199</v>
+      </c>
+      <c r="B42" s="45" t="s">
         <v>200</v>
-      </c>
-      <c r="B42" s="45" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="45" t="s">
+        <v>201</v>
+      </c>
+      <c r="B43" s="45" t="s">
         <v>202</v>
-      </c>
-      <c r="B43" s="45" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="45" t="s">
+        <v>203</v>
+      </c>
+      <c r="B44" s="45" t="s">
         <v>204</v>
-      </c>
-      <c r="B44" s="45" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="45" t="s">
+        <v>205</v>
+      </c>
+      <c r="B45" s="45" t="s">
         <v>206</v>
-      </c>
-      <c r="B45" s="45" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="45" t="s">
+        <v>207</v>
+      </c>
+      <c r="B46" s="45" t="s">
         <v>208</v>
-      </c>
-      <c r="B46" s="45" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="45" t="s">
+        <v>209</v>
+      </c>
+      <c r="B47" s="45" t="s">
         <v>210</v>
-      </c>
-      <c r="B47" s="45" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="45" t="s">
+        <v>211</v>
+      </c>
+      <c r="B48" s="45" t="s">
         <v>212</v>
-      </c>
-      <c r="B48" s="45" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="45" t="s">
+        <v>213</v>
+      </c>
+      <c r="B49" s="45" t="s">
         <v>214</v>
-      </c>
-      <c r="B49" s="45" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="45" t="s">
+        <v>215</v>
+      </c>
+      <c r="B50" s="45" t="s">
         <v>216</v>
-      </c>
-      <c r="B50" s="45" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="45" t="s">
+        <v>217</v>
+      </c>
+      <c r="B51" s="45" t="s">
         <v>218</v>
-      </c>
-      <c r="B51" s="45" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="45" t="s">
+        <v>219</v>
+      </c>
+      <c r="B52" s="45" t="s">
         <v>220</v>
-      </c>
-      <c r="B52" s="45" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="45" t="s">
+        <v>221</v>
+      </c>
+      <c r="B53" s="45" t="s">
         <v>222</v>
-      </c>
-      <c r="B53" s="45" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="45" t="s">
+        <v>223</v>
+      </c>
+      <c r="B54" s="45" t="s">
         <v>224</v>
-      </c>
-      <c r="B54" s="45" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="45" t="s">
+        <v>225</v>
+      </c>
+      <c r="B55" s="45" t="s">
         <v>226</v>
-      </c>
-      <c r="B55" s="45" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="45" t="s">
+        <v>227</v>
+      </c>
+      <c r="B56" s="45" t="s">
         <v>228</v>
-      </c>
-      <c r="B56" s="45" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="45" t="s">
+        <v>229</v>
+      </c>
+      <c r="B57" s="45" t="s">
         <v>230</v>
-      </c>
-      <c r="B57" s="45" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="45" t="s">
+        <v>231</v>
+      </c>
+      <c r="B58" s="45" t="s">
         <v>232</v>
-      </c>
-      <c r="B58" s="45" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="45" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B59" s="45" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>